<commit_message>
Debug BASIC file directly(still experimental)
-d option: generate c++ file with debug infomation for using GDB
</commit_message>
<xml_diff>
--- a/others/VSCode-For-FreeBASIC.xlsx
+++ b/others/VSCode-For-FreeBASIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HongbinHan\Documents\GitHub\Kaya-BASIC\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F27B7D-5146-4216-8D85-EC9996733FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD23C22-307E-4CA9-B842-3BB3A83C3FA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B4019E9-5368-45CF-99B0-E2E31AB50AE4}"/>
   </bookViews>
@@ -154,10 +154,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>click the test.bas file and enjon write codes with code completion.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Debug</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -166,19 +162,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>because the C/C++ extension can only set breakpoint the c/c++ file, we need to change Debug settings.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>F5 to run/debug, enjon GDB debugging.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>https://github.com/kankouhin/Kaya-BASIC/blob/master/others/FreeBASIC.zip</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>this sample can download from:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>click the test.bas file and enjoy write codes with code completion.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>because the C/C++ extension can only set breakpoint to c/c++ file, we need to change Debug settings.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F5 to run/debug, enjoy GDB debugging.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2984,12 +2984,12 @@
     </row>
     <row r="116" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C116" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" spans="3:9" x14ac:dyDescent="0.45">
       <c r="D117" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="118" spans="3:9" x14ac:dyDescent="0.45">
@@ -3015,7 +3015,7 @@
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C182" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="204" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -3023,22 +3023,22 @@
         <v>28</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C205" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="222" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C222" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="241" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C241" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>